<commit_message>
Sync Forms export and update outputs
</commit_message>
<xml_diff>
--- a/PeerGrading/Input/form_exports/forms_responses.xlsx
+++ b/PeerGrading/Input/form_exports/forms_responses.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="1" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29816"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0619ABFA-B3B8-4DB1-9606-ED6E60BE04FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_9248711583CF9423E851EEDB953E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D52B2DC0-EF3E-4429-BF5D-14582A79FDA5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -44,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
   <si>
     <t>ResponseId</t>
   </si>
@@ -103,6 +98,12 @@
     <t>testtt</t>
   </si>
   <si>
+    <t>utcNow()</t>
+  </si>
+  <si>
+    <t>achille.desbrieres@uzh.ch</t>
+  </si>
+  <si>
     <t>test2222</t>
   </si>
   <si>
@@ -157,17 +158,29 @@
     <t>2026-02-20T09:58:26.8961547Z</t>
   </si>
   <si>
-    <t>ajaysathish.shenoy@uzh.ch</t>
-  </si>
-  <si>
-    <t>benjaminlucasde.gorgey@uzh.ch</t>
+    <t>Steven Thomas	Uvakov</t>
+  </si>
+  <si>
+    <t>testttt</t>
+  </si>
+  <si>
+    <t>2026-02-22T19:44:21.8423287Z</t>
+  </si>
+  <si>
+    <t>Erik	Macniel</t>
+  </si>
+  <si>
+    <t>testestest</t>
+  </si>
+  <si>
+    <t>2026-02-22T19:45:42.8842352Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,10 +190,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,17 +211,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{69BDF735-796B-4CD7-BB8A-DFB7136645AF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -226,8 +236,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}" name="Responses" displayName="Responses" ref="A1:N8" totalsRowShown="0">
-  <autoFilter ref="A1:N8" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}" name="Responses" displayName="Responses" ref="A1:N10" totalsRowShown="0">
+  <autoFilter ref="A1:N10" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{FB89DE1D-4C11-4761-8D11-788CCF566045}" name="ResponseId"/>
     <tableColumn id="2" xr3:uid="{EAB2BAF6-0686-4B33-A477-A5DC980B3E48}" name="SubmittedAt"/>
@@ -249,9 +259,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +299,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -395,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -537,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -545,24 +555,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
@@ -644,18 +654,18 @@
         <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -664,72 +674,72 @@
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>17</v>
       </c>
       <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
@@ -740,157 +750,245 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K5" t="s">
         <v>17</v>
       </c>
       <c r="L5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" t="s">
-        <v>35</v>
-      </c>
       <c r="N8" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>46075.822465277779</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>46075.82340277778</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -905,9 +1003,5 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28D4E43F-BCF1-4B87-8DDD-890AC7C5379F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28D4E43F-BCF1-4B87-8DDD-890AC7C5379F}"/>
 </file>
</xml_diff>

<commit_message>
Sync Forms export and update outputs (#6)
Co-authored-by: aydinarda <120125109+aydinarda@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PeerGrading/Input/form_exports/forms_responses.xlsx
+++ b/PeerGrading/Input/form_exports/forms_responses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29816"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_9248711583CF9423E851EEDB953E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{755844A7-6771-4ED9-8593-024815D32592}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_9248711583CF9423E851EEDB953E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EDB5DA4-E265-484E-8EB5-D9FDE24E95C9}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="48">
   <si>
     <t>ResponseId</t>
   </si>
@@ -177,13 +177,20 @@
   </si>
   <si>
     <t>2026-03-22T19:45:42.8842352Z</t>
+  </si>
+  <si>
+    <t>anargyros.megalios@uzh.ch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan-Akim Albert Reimer
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +202,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,10 +230,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,8 +256,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}" name="Responses" displayName="Responses" ref="A1:N11" totalsRowShown="0">
-  <autoFilter ref="A1:N11" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}" name="Responses" displayName="Responses" ref="A1:N14" totalsRowShown="0">
+  <autoFilter ref="A1:N14" xr:uid="{6FE71E5D-2FC8-4A7C-9471-2FA3E1955E04}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{FB89DE1D-4C11-4761-8D11-788CCF566045}" name="ResponseId"/>
     <tableColumn id="2" xr3:uid="{EAB2BAF6-0686-4B33-A477-A5DC980B3E48}" name="SubmittedAt"/>
@@ -558,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,6 +1052,129 @@
         <v>45</v>
       </c>
     </row>
+    <row r="12" spans="1:14" ht="15.75">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="48.75">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="48.75">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Sync Forms export and update outputs (#7)
Co-authored-by: aydinarda <120125109+aydinarda@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PeerGrading/Input/form_exports/forms_responses.xlsx
+++ b/PeerGrading/Input/form_exports/forms_responses.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29816"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_9248711583CF9423E851EEDB953E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EDB5DA4-E265-484E-8EB5-D9FDE24E95C9}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="11_9248711583CF9423E851EEDB953E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD62D8FE-2D31-4446-8DBD-4A035E36E887}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,8 +234,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -578,7 +578,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1025,13 +1025,13 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Sync Forms export and update outputs (#4)
Co-authored-by: RenjieCui <71599592+RenjieCui@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/PeerGrading/Input/form_exports/forms_responses.xlsx
+++ b/PeerGrading/Input/form_exports/forms_responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uzh-my.sharepoint.com/personal/renjie_cui_business_uzh_ch/Documents/PeerGrading/Input/form_exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{9C3C9BE7-B8B4-430B-A3DC-C1A29F196D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C17583C3-7C51-445A-A15F-7B006593C733}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{9C3C9BE7-B8B4-430B-A3DC-C1A29F196D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34303232-B81A-4FBB-9951-0A8009860673}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17280" yWindow="-16200" windowWidth="29010" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2799" uniqueCount="352">
   <si>
     <t>Responseid</t>
   </si>
@@ -1083,6 +1083,15 @@
   </si>
   <si>
     <t>ReceivedAtUTC</t>
+  </si>
+  <si>
+    <t>2026-02-26T14:28:08.5054068Z</t>
+  </si>
+  <si>
+    <t>The presentation was not entirely effective because his voice often faded, and the responses to questions were not sufficiently comprehensive.</t>
+  </si>
+  <si>
+    <t>2026-02-26T14:28:08.5054510Z</t>
   </si>
 </sst>
 </file>
@@ -1118,11 +1127,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1181,8 +1191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="OfficeForms.Table" displayName="OfficeForms.Table" ref="A1:N253" totalsRowShown="0">
-  <autoFilter ref="A1:N253" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="responses" displayName="responses" ref="A1:N254" totalsRowShown="0">
+  <autoFilter ref="A1:N254" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Responseid" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="SubmittedAt"/>
@@ -1500,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N253"/>
+  <dimension ref="A1:N254"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:N253"/>
+    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
+      <selection activeCell="A254" sqref="A254:XFD254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12643,6 +12653,50 @@
         <v>46077.444178240701</v>
       </c>
     </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A254" s="4">
+        <v>255</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D254" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F254" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G254" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H254" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I254" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J254" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K254" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L254" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M254" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="N254" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>